<commit_message>
TC-24 added in TestPlan tab
added method verifyReleaseUpdateNotification(String releaseId),getLoggedInUserName() in IndividualReleasePage

added data for TC024
</commit_message>
<xml_diff>
--- a/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
+++ b/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\testPlanTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7614E411-1FDD-43D3-9C65-B6B45F00B786}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29BB686-89D7-465D-B67E-470252C87A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="2320" windowWidth="14400" windowHeight="7270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc002" sheetId="2" r:id="rId1"/>
@@ -23,11 +23,12 @@
     <sheet name="tc010" sheetId="7" r:id="rId8"/>
     <sheet name="tc011" sheetId="8" r:id="rId9"/>
     <sheet name="tc020" sheetId="13" r:id="rId10"/>
-    <sheet name="tc013" sheetId="6" r:id="rId11"/>
-    <sheet name="tc014" sheetId="9" r:id="rId12"/>
-    <sheet name="tc015" sheetId="11" r:id="rId13"/>
-    <sheet name="tc018" sheetId="15" r:id="rId14"/>
-    <sheet name="tc019" sheetId="14" r:id="rId15"/>
+    <sheet name="tc024" sheetId="17" r:id="rId11"/>
+    <sheet name="tc013" sheetId="6" r:id="rId12"/>
+    <sheet name="tc014" sheetId="9" r:id="rId13"/>
+    <sheet name="tc015" sheetId="11" r:id="rId14"/>
+    <sheet name="tc018" sheetId="15" r:id="rId15"/>
+    <sheet name="tc019" sheetId="14" r:id="rId16"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
   <si>
     <t>projectName</t>
   </si>
@@ -159,6 +160,12 @@
   </si>
   <si>
     <t>STG- SPARK Modernization</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Release update notoification 09-01-2026</t>
+  </si>
+  <si>
+    <t>Status</t>
   </si>
 </sst>
 </file>
@@ -567,7 +574,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2B23743E-2A7E-44B5-B321-E0E01B81F69B}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -603,7 +610,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -633,6 +640,47 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB47FFB-5701-40BD-8651-2BE6A7946C21}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="30.453125" customWidth="1"/>
+    <col min="2" max="2" width="34.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629D3112-3371-4BF7-8E34-7EF404484B7A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -674,7 +722,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB833951-6912-4EC9-ACE3-69E572816D68}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -723,7 +771,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0525B04B-FF17-434F-88AB-61B4785D0097}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -772,7 +820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E586B257-6C9A-4EFD-A8EB-37EC5826DD12}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -797,7 +845,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAB45CC-E342-4AFE-8447-7AB01267C45A}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>

<commit_message>
TC-25 added in TestPlan tab
added method verifyCycleUpdateNotification(String cycleId),getLoggedInUserName() in IndividualTestCyclePage

added data for TC025
</commit_message>
<xml_diff>
--- a/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
+++ b/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MohitAman\Desktop\UAT_NEXTNEXT_BLAZE_FRAMEWORK_AUTO\testData\testPlanTabTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C29BB686-89D7-465D-B67E-470252C87A76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1D22916-0AA3-4CE0-A4E9-729B24F74A71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="tc002" sheetId="2" r:id="rId1"/>
@@ -24,11 +24,13 @@
     <sheet name="tc011" sheetId="8" r:id="rId9"/>
     <sheet name="tc020" sheetId="13" r:id="rId10"/>
     <sheet name="tc024" sheetId="17" r:id="rId11"/>
-    <sheet name="tc013" sheetId="6" r:id="rId12"/>
-    <sheet name="tc014" sheetId="9" r:id="rId13"/>
-    <sheet name="tc015" sheetId="11" r:id="rId14"/>
-    <sheet name="tc018" sheetId="15" r:id="rId15"/>
-    <sheet name="tc019" sheetId="14" r:id="rId16"/>
+    <sheet name="tc025" sheetId="18" r:id="rId12"/>
+    <sheet name="tc026" sheetId="19" r:id="rId13"/>
+    <sheet name="tc013" sheetId="6" r:id="rId14"/>
+    <sheet name="tc014" sheetId="9" r:id="rId15"/>
+    <sheet name="tc015" sheetId="11" r:id="rId16"/>
+    <sheet name="tc018" sheetId="15" r:id="rId17"/>
+    <sheet name="tc019" sheetId="14" r:id="rId18"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -40,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="50">
   <si>
     <t>projectName</t>
   </si>
@@ -162,10 +164,34 @@
     <t>STG- SPARK Modernization</t>
   </si>
   <si>
-    <t xml:space="preserve"> Release update notoification 09-01-2026</t>
-  </si>
-  <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Tesplaname</t>
+  </si>
+  <si>
+    <t>des</t>
+  </si>
+  <si>
+    <t>planned</t>
+  </si>
+  <si>
+    <t>Cyclename</t>
+  </si>
+  <si>
+    <t>Suitename</t>
+  </si>
+  <si>
+    <t>Cyle update notification 09-01-2026</t>
+  </si>
+  <si>
+    <t>Suite update notification 09-01-2026</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Release update notification 09-01-2026</t>
+  </si>
+  <si>
+    <t>Desc</t>
   </si>
 </sst>
 </file>
@@ -643,8 +669,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BB47FFB-5701-40BD-8651-2BE6A7946C21}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -661,7 +687,7 @@
         <v>22</v>
       </c>
       <c r="C1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -669,7 +695,7 @@
         <v>2</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>40</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>34</v>
@@ -681,6 +707,108 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B27E3B84-2B56-4E59-9275-679545FE5609}">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" width="22.81640625" customWidth="1"/>
+    <col min="2" max="2" width="34.6328125" customWidth="1"/>
+    <col min="3" max="3" width="31.1796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC2DFA25-D2D8-4EB2-9C83-09FF0B980780}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="2" max="2" width="38.54296875" customWidth="1"/>
+    <col min="3" max="3" width="31.6328125" customWidth="1"/>
+    <col min="4" max="4" width="38.36328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629D3112-3371-4BF7-8E34-7EF404484B7A}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -722,7 +850,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AB833951-6912-4EC9-ACE3-69E572816D68}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -771,7 +899,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0525B04B-FF17-434F-88AB-61B4785D0097}">
   <dimension ref="A1:D2"/>
   <sheetViews>
@@ -820,7 +948,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E586B257-6C9A-4EFD-A8EB-37EC5826DD12}">
   <dimension ref="A1:A2"/>
   <sheetViews>
@@ -845,7 +973,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAB45CC-E342-4AFE-8447-7AB01267C45A}">
   <dimension ref="A1:B2"/>
   <sheetViews>

</xml_diff>